<commit_message>
Misc changes: code review bug fixes
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SD_Summary_Template-v2.xlsx
+++ b/application/controllers/excel-templates/SD_Summary_Template-v2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-dev/application/controllers/excel-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="snapdeal_leads__7" localSheetId="0">Sheet1!$A$1:$T$1</definedName>
+    <definedName name="snapdeal_leads__7" localSheetId="0">Sheet1!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -68,13 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
-  <si>
-    <t>Referred_Date_and_Time</t>
-  </si>
-  <si>
-    <t>Sub_Order_ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Brand</t>
   </si>
@@ -85,15 +79,6 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Product_Type</t>
-  </si>
-  <si>
-    <t>Customer_Name</t>
-  </si>
-  <si>
-    <t>Customer_Address</t>
-  </si>
-  <si>
     <t>Pincode</t>
   </si>
   <si>
@@ -103,33 +88,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>CRM_Remarks_SR_No</t>
-  </si>
-  <si>
-    <t>Status_by_247around</t>
-  </si>
-  <si>
-    <t>Remarks_by_247around</t>
-  </si>
-  <si>
-    <t>Scheduled_Appointment_DateDDMMYYYY</t>
-  </si>
-  <si>
-    <t>Scheduled_Appointment_Time</t>
-  </si>
-  <si>
-    <t>Rating_Stars</t>
-  </si>
-  <si>
-    <t>Status_by_Snapdeal</t>
-  </si>
-  <si>
-    <t>Remarks_by_Snapdeal</t>
-  </si>
-  <si>
-    <t>Final_Status</t>
-  </si>
-  <si>
     <t>{bd:create_date}</t>
   </si>
   <si>
@@ -179,6 +137,39 @@
   </si>
   <si>
     <t>{bd:booking_timeslot}</t>
+  </si>
+  <si>
+    <t>Reference Date</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Customer Address</t>
+  </si>
+  <si>
+    <t>247around Booking ID</t>
+  </si>
+  <si>
+    <t>Status - Level 1</t>
+  </si>
+  <si>
+    <t>Status - Level 2</t>
+  </si>
+  <si>
+    <t>Booking Date</t>
+  </si>
+  <si>
+    <t>Booking Timeslot</t>
+  </si>
+  <si>
+    <t>Customer Rating</t>
   </si>
 </sst>
 </file>
@@ -222,9 +213,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,150 +505,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.83203125" customWidth="1"/>
-    <col min="14" max="14" width="28.83203125" customWidth="1"/>
-    <col min="15" max="15" width="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16" style="2" customWidth="1"/>
+    <col min="15" max="15" width="19.83203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="M2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="P5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
snapdeal summary report CSV
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SD_Summary_Template-v2.xlsx
+++ b/application/controllers/excel-templates/SD_Summary_Template-v2.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="snapdeal_leads__7" vbProcedure="false">Sheet1!$C$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="snapdeal_leads__7" vbProcedure="false">Sheet1!$C$1:$L$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Scheduled Appointment Date(DD/MM/YYYY)</t>
   </si>
@@ -46,21 +46,9 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pincode</t>
-  </si>
-  <si>
     <t xml:space="preserve">City</t>
   </si>
   <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
     <t xml:space="preserve">247around Booking ID</t>
   </si>
   <si>
@@ -73,9 +61,6 @@
     <t xml:space="preserve">Final Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer Rating</t>
-  </si>
-  <si>
     <t xml:space="preserve">{bd:booking_date}</t>
   </si>
   <si>
@@ -97,21 +82,9 @@
     <t xml:space="preserve">{bd:description}</t>
   </si>
   <si>
-    <t xml:space="preserve">{bd:name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{bd:home_address}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{bd:pincode}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{bd:city}</t>
   </si>
   <si>
-    <t xml:space="preserve">{bd:phone_number}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{bd:booking_id}</t>
   </si>
   <si>
@@ -122,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">{bd:partner_internal_status}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{bd:rating_stars}</t>
   </si>
 </sst>
 </file>
@@ -134,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -164,12 +134,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,7 +191,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,30 +212,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="57.7185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.8333333333333"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.7592592592593"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="59.1888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1019" min="13" style="1" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,73 +271,48 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get State from india pincode file, changes in penalty funtion, BUG in allot source, partner edit booking form, add status in Pending page, Send partner summary booking, vendor add/edit function
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SD_Summary_Template-v2.xlsx
+++ b/application/controllers/excel-templates/SD_Summary_Template-v2.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="snapdeal_leads__7" vbProcedure="false">Sheet1!$C$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="snapdeal_leads__7" vbProcedure="false">Sheet1!$C$1:$L$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Scheduled Appointment Date(DD/MM/YYYY)</t>
   </si>
@@ -46,21 +46,9 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pincode</t>
-  </si>
-  <si>
     <t xml:space="preserve">City</t>
   </si>
   <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
     <t xml:space="preserve">247around Booking ID</t>
   </si>
   <si>
@@ -73,9 +61,6 @@
     <t xml:space="preserve">Final Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer Rating</t>
-  </si>
-  <si>
     <t xml:space="preserve">{bd:booking_date}</t>
   </si>
   <si>
@@ -97,21 +82,9 @@
     <t xml:space="preserve">{bd:description}</t>
   </si>
   <si>
-    <t xml:space="preserve">{bd:name}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{bd:home_address}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{bd:pincode}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{bd:city}</t>
   </si>
   <si>
-    <t xml:space="preserve">{bd:phone_number}</t>
-  </si>
-  <si>
     <t xml:space="preserve">{bd:booking_id}</t>
   </si>
   <si>
@@ -122,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">{bd:partner_internal_status}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{bd:rating_stars}</t>
   </si>
 </sst>
 </file>
@@ -134,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -164,12 +134,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,7 +191,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,30 +212,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="57.7185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="66.8333333333333"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.7592592592593"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="59.1888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1019" min="13" style="1" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,73 +271,48 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>